<commit_message>
them hoat dong truoc cho cac code module
</commit_message>
<xml_diff>
--- a/Documents/Activity_Table.xlsx
+++ b/Documents/Activity_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\HQN-Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\HQN-Team\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB03CEA1-299F-4FA5-9DFA-382350A5A6FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B5E265-423E-41B3-BE6E-FA672DF4792E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="2655" windowWidth="13320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1455" windowWidth="13320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -60,12 +60,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Thiết kế giao diện</t>
-  </si>
-  <si>
-    <t>Xây dựng giao diện</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -141,16 +135,16 @@
     <t>Hoàn chỉnh giao diện</t>
   </si>
   <si>
-    <t>I, J, K, L, M, N, O</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>P, Q</t>
-  </si>
-  <si>
     <t>Hoàn thiện sản phẩm</t>
+  </si>
+  <si>
+    <t>Thiết kế và xây dựng giao diện</t>
+  </si>
+  <si>
+    <t>D, G</t>
+  </si>
+  <si>
+    <t>H, I, J, K, L, M, N</t>
   </si>
 </sst>
 </file>
@@ -246,7 +240,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,6 +261,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -365,8 +362,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A2:D19" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" headerRowCellStyle="Heading 2">
-  <autoFilter ref="A2:D19" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A2:D18" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A2:D18" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="3" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hoạt động" dataDxfId="2"/>
@@ -643,7 +640,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +692,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -709,7 +706,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="6">
         <v>6</v>
@@ -723,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -734,13 +731,13 @@
     </row>
     <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>10</v>
@@ -748,171 +745,163 @@
     </row>
     <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C9" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6">
         <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6">
         <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C15" s="6">
         <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C16" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="A19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Thêm các biểu đồ và chỉnh sửa Activity table
</commit_message>
<xml_diff>
--- a/Documents/Activity_Table.xlsx
+++ b/Documents/Activity_Table.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\HQN-Team\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COSMOS\STUDY\Sophomore\HKII\PBL3\HQN-Team\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B5E265-423E-41B3-BE6E-FA672DF4792E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1455" windowWidth="13320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1452" windowWidth="13320" windowHeight="11388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -144,13 +143,19 @@
     <t>D, G</t>
   </si>
   <si>
-    <t>H, I, J, K, L, M, N</t>
+    <t>K, L, N</t>
+  </si>
+  <si>
+    <t>Nhân lực</t>
+  </si>
+  <si>
+    <t>STT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -240,7 +245,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,11 +265,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -273,7 +287,24 @@
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <sz val="13"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -362,13 +393,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A2:D18" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" headerRowCellStyle="Heading 2">
-  <autoFilter ref="A2:D18" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="3" dataCellStyle="Good"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hoạt động" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Số ngày" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Hoạt động trước" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B2:F18" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B2:F18"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="ID" dataDxfId="7"/>
+    <tableColumn id="2" name="Hoạt động" dataDxfId="6"/>
+    <tableColumn id="3" name="Số ngày" dataDxfId="5"/>
+    <tableColumn id="4" name="Hoạt động trước" dataDxfId="4"/>
+    <tableColumn id="5" name="Nhân lực" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:A18" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A2:A18"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="STT" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -636,281 +678,388 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="F2" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="F4" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="6">
+      <c r="D5" s="6">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="F9" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6">
+      <c r="D10" s="6">
         <v>2</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6">
+      <c r="D11" s="6">
         <v>2</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6">
+      <c r="D12" s="6">
         <v>2</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="E12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6">
+      <c r="D13" s="6">
         <v>2</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="E13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6">
+      <c r="D14" s="6">
         <v>2</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="E14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="6">
+      <c r="D15" s="6">
         <v>2</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="E15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="F17" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
+      <c r="F18" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="7"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sua ngay xay dung csdl trong activity table Sua so do ADM Them so do AON Them bang thong ke nhan luc Them duong gang Xoa bieud o Grantt va bieu do phu tai cu
</commit_message>
<xml_diff>
--- a/Documents/Activity_Table.xlsx
+++ b/Documents/Activity_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -150,13 +150,40 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>Tên nhân lực</t>
+  </si>
+  <si>
+    <t>1. Huỳnh Phú Quý</t>
+  </si>
+  <si>
+    <t>3. Huỳnh Phú Quý</t>
+  </si>
+  <si>
+    <t>1. Hoàng Quang Hùng
+2. Vũ Xuân Nguyên</t>
+  </si>
+  <si>
+    <t>2. Vũ Xuân Nguyên</t>
+  </si>
+  <si>
+    <t>1. Vũ Xuân Nguyên</t>
+  </si>
+  <si>
+    <t>1. Hoàng Quang Hùng
+2. Vũ Xuân Nguyên
+3. Huỳnh Phú Quý</t>
+  </si>
+  <si>
+    <t>1. Hoàng Quang Hùng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +224,13 @@
       <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,18 +279,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -268,17 +293,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -287,23 +330,43 @@
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <sz val="13"/>
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -321,7 +384,7 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -339,7 +402,7 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -360,7 +423,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -375,9 +438,6 @@
           <color theme="4" tint="0.499984740745262"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,24 +453,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B2:F18" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B2:F18"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="7"/>
-    <tableColumn id="2" name="Hoạt động" dataDxfId="6"/>
-    <tableColumn id="3" name="Số ngày" dataDxfId="5"/>
-    <tableColumn id="4" name="Hoạt động trước" dataDxfId="4"/>
-    <tableColumn id="5" name="Nhân lực" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B2:G18" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="12" tableBorderDxfId="11" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B2:G18"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Hoạt động" dataDxfId="9"/>
+    <tableColumn id="3" name="Số ngày" dataDxfId="8"/>
+    <tableColumn id="4" name="Hoạt động trước" dataDxfId="7"/>
+    <tableColumn id="5" name="Nhân lực" dataDxfId="6"/>
+    <tableColumn id="6" name="Tên nhân lực" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:A18" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:A18" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowCellStyle="Heading 2">
   <autoFilter ref="A2:A18"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="STT" dataDxfId="1"/>
+    <tableColumn id="1" name="STT" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -679,377 +740,428 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" customWidth="1"/>
+    <col min="1" max="2" width="5.44140625" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:7" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="G2" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="12">
+        <v>14</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="14">
+        <v>6</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="14">
+        <v>3</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="F7" s="13">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="14">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="E9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="B10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="E10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="14">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="14">
+        <v>2</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="14">
+        <v>2</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="14">
+        <v>2</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>14</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="14">
+        <v>1</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="6">
-        <v>6</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="G16" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>15</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="13">
         <v>3</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="6">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="G17" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="6">
-        <v>2</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6">
-        <v>2</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="6">
-        <v>2</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="6">
-        <v>2</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="11">
+      <c r="F18" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update ngay trong activity table
</commit_message>
<xml_diff>
--- a/Documents/Activity_Table.xlsx
+++ b/Documents/Activity_Table.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COSMOS\STUDY\Sophomore\HKII\PBL3\HQN-Team\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\HQN-Team\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFBEE2E-9A4F-4CBD-8706-1A4D34960E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1452" windowWidth="13320" windowHeight="11388"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -171,15 +181,12 @@
   </si>
   <si>
     <t>1. Hoàng Quang Hùng</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -317,14 +324,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -333,10 +340,7 @@
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -459,26 +463,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B2:H18" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B2:H18"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="ID" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Hoạt động" dataDxfId="8"/>
-    <tableColumn id="3" name="Số ngày" dataDxfId="7"/>
-    <tableColumn id="4" name="Hoạt động trước" dataDxfId="6"/>
-    <tableColumn id="5" name="Nhân lực" dataDxfId="5"/>
-    <tableColumn id="6" name="Tên nhân lực" dataDxfId="4"/>
-    <tableColumn id="7" name="Column1" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="B2:G18" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B2:G18" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hoạt động" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Số ngày" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Hoạt động trước" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nhân lực" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tên nhân lực" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:A18" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Heading 2">
-  <autoFilter ref="A2:A18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A2:A18" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A2:A18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="STT" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="STT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -746,34 +749,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5.44140625" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="1" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
@@ -795,11 +798,9 @@
       <c r="G2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -821,9 +822,9 @@
       <c r="G3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -845,9 +846,9 @@
       <c r="G4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -869,9 +870,9 @@
       <c r="G5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -893,9 +894,9 @@
       <c r="G6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -917,9 +918,9 @@
       <c r="G7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -941,9 +942,9 @@
       <c r="G8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -965,9 +966,9 @@
       <c r="G9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -989,9 +990,9 @@
       <c r="G10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -1013,9 +1014,9 @@
       <c r="G11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -1037,9 +1038,9 @@
       <c r="G12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -1061,9 +1062,9 @@
       <c r="G13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -1085,9 +1086,9 @@
       <c r="G14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -1109,9 +1110,9 @@
       <c r="G15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -1122,7 +1123,7 @@
         <v>24</v>
       </c>
       <c r="D16" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>39</v>
@@ -1133,9 +1134,9 @@
       <c r="G16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>36</v>
       </c>
       <c r="D17" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>32</v>
@@ -1157,9 +1158,9 @@
       <c r="G17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>33</v>
@@ -1181,9 +1182,9 @@
       <c r="G18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>

</xml_diff>

<commit_message>
bo sung ten nhan luc Activity_Table
</commit_message>
<xml_diff>
--- a/Documents/Activity_Table.xlsx
+++ b/Documents/Activity_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\HQN-Team\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFBEE2E-9A4F-4CBD-8706-1A4D34960E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7960ABA6-E02C-428B-9DB7-543FA1AD248C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="825" windowWidth="13320" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,7 +753,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H8" s="14"/>
     </row>

</xml_diff>

<commit_message>
Them muc A cho Activity_Tabe
</commit_message>
<xml_diff>
--- a/Documents/Activity_Table.xlsx
+++ b/Documents/Activity_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\HQN-Team\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7960ABA6-E02C-428B-9DB7-543FA1AD248C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9C8DED-874A-4DDC-8602-FDD60D12BAD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="825" windowWidth="13320" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Thiết kế và xây dựng giao diện</t>
-  </si>
-  <si>
-    <t>D, G</t>
   </si>
   <si>
     <t>K, L, N</t>
@@ -181,13 +178,22 @@
   </si>
   <si>
     <t>1. Hoàng Quang Hùng</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Khảo sát, phân tích, phát thảo và thiết kế hệ thống</t>
+  </si>
+  <si>
+    <t>E, G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,13 +218,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -237,17 +236,12 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -277,27 +271,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
@@ -306,22 +290,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -333,19 +311,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
+  <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -409,27 +413,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thick">
           <color theme="4"/>
@@ -463,25 +446,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="B2:G18" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B2:G18" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="B2:G19" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B2:G19" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hoạt động" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Số ngày" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Hoạt động trước" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nhân lực" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tên nhân lực" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hoạt động" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Số ngày" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Hoạt động trước" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nhân lực" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tên nhân lực" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A2:A18" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowCellStyle="Heading 2">
-  <autoFilter ref="A2:A18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A2:A19" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A2:A19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="STT" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="STT" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -753,7 +736,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,428 +750,445 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" ht="50.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="8">
+        <v>10</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8">
+        <v>14</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8">
+        <v>6</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="D3" s="11">
+      <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" ht="33" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="B12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="12">
+      <c r="E12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="8">
         <v>2</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="E13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>13</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="8">
+        <v>2</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>15</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="8">
+        <v>4</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="13">
-        <v>6</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="12">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" ht="33" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="12">
-        <v>2</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>5</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="G17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>16</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="8">
         <v>3</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="E18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="8">
+        <v>3</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>6</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="12">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="14"/>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <v>17</v>
       </c>
-      <c r="D9" s="13">
-        <v>2</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="12">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>8</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="13">
-        <v>2</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="12">
-        <v>1</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="B19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="8">
+        <v>3</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="7">
+        <v>3</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="14"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="13">
-        <v>2</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="12">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>10</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="13">
-        <v>2</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>11</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="13">
-        <v>2</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="12">
-        <v>1</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="13">
-        <v>2</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="12">
-        <v>1</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>13</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="13">
-        <v>2</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="12">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>14</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="13">
-        <v>4</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="12">
-        <v>3</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="14"/>
-    </row>
-    <row r="17" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>15</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="13">
-        <v>3</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="12">
-        <v>3</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>16</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="13">
-        <v>3</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="12">
-        <v>3</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="14"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Cap nhat Bao cao
</commit_message>
<xml_diff>
--- a/Documents/Activity_Table.xlsx
+++ b/Documents/Activity_Table.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\HQN-Team\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COSMOS\STUDY\Sophomore\HKII\PBL3\HQN-Team\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9C8DED-874A-4DDC-8602-FDD60D12BAD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -192,7 +191,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -308,14 +307,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -329,27 +328,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -413,6 +391,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thick">
           <color theme="4"/>
@@ -446,25 +445,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="B2:G19" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B2:G19" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B2:G19" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B2:G19"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hoạt động" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Số ngày" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Hoạt động trước" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nhân lực" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tên nhân lực" dataDxfId="5"/>
+    <tableColumn id="1" name="ID" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Hoạt động" dataDxfId="7"/>
+    <tableColumn id="3" name="Số ngày" dataDxfId="6"/>
+    <tableColumn id="4" name="Hoạt động trước" dataDxfId="5"/>
+    <tableColumn id="5" name="Nhân lực" dataDxfId="4"/>
+    <tableColumn id="6" name="Tên nhân lực" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A2:A19" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0" headerRowCellStyle="Heading 2">
-  <autoFilter ref="A2:A19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:A19" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A2:A19"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="STT" dataDxfId="1"/>
+    <tableColumn id="1" name="STT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -732,34 +731,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="5.42578125" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="1" max="2" width="5.44140625" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
@@ -783,7 +782,7 @@
       </c>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" ht="50.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="51" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -807,7 +806,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -826,12 +825,12 @@
       <c r="F4" s="8">
         <v>1</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -850,12 +849,12 @@
       <c r="F5" s="8">
         <v>2</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>43</v>
       </c>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -874,16 +873,16 @@
       <c r="F6" s="8">
         <v>1</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>42</v>
       </c>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -898,16 +897,16 @@
       <c r="F7" s="8">
         <v>2</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>43</v>
       </c>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -917,21 +916,21 @@
         <v>3</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F8" s="8">
         <v>1</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>44</v>
       </c>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -946,16 +945,16 @@
       <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -970,16 +969,16 @@
       <c r="F10" s="8">
         <v>1</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -994,16 +993,16 @@
       <c r="F11" s="8">
         <v>1</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>44</v>
       </c>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1018,16 +1017,16 @@
       <c r="F12" s="8">
         <v>1</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>42</v>
       </c>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1042,16 +1041,16 @@
       <c r="F13" s="8">
         <v>1</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>44</v>
       </c>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1066,16 +1065,16 @@
       <c r="F14" s="8">
         <v>1</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>46</v>
       </c>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>13</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1090,16 +1089,16 @@
       <c r="F15" s="8">
         <v>1</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>42</v>
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>14</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1114,16 +1113,16 @@
       <c r="F16" s="8">
         <v>1</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="12" t="s">
         <v>46</v>
       </c>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1138,16 +1137,16 @@
       <c r="F17" s="8">
         <v>3</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="12" t="s">
         <v>45</v>
       </c>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>16</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1162,12 +1161,12 @@
       <c r="F18" s="8">
         <v>3</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>45</v>
       </c>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>17</v>
       </c>

</xml_diff>